<commit_message>
435  452 1024 64
</commit_message>
<xml_diff>
--- a/leetcode/00_already.xlsx
+++ b/leetcode/00_already.xlsx
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A104"/>
+  <dimension ref="A1:A108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -891,6 +891,26 @@
         <v>518</v>
       </c>
     </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>